<commit_message>
Numerical example for paper. Better data organizing
</commit_message>
<xml_diff>
--- a/data/APS.dat.xlsx
+++ b/data/APS.dat.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\modelo-aps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Dropbox\01-UFMG\02-Pesquisa\_2023-CNPq-21-2023\modelo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54CEBFC6-B215-48ED-A26C-F942C75CA9B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A118AAE-F472-4807-B144-0E13D0886BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29490" yWindow="2025" windowWidth="27825" windowHeight="13680" activeTab="1" xr2:uid="{25D375F3-B3FF-492F-B94B-D88A37ADD5E2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{25D375F3-B3FF-492F-B94B-D88A37ADD5E2}"/>
   </bookViews>
   <sheets>
     <sheet name="LS" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="758">
   <si>
     <t>313760105000002</t>
   </si>
@@ -2228,17 +2228,144 @@
   </si>
   <si>
     <t>eMulti (1/9)</t>
+  </si>
+  <si>
+    <t>Cvar/pop</t>
+  </si>
+  <si>
+    <t>Custo fixo (adm):</t>
+  </si>
+  <si>
+    <t>(R$/ano)</t>
+  </si>
+  <si>
+    <t>Fonte: https://cbc2022.abcustos.org.br/rest/artigo/98/semFolhaDeRosto/pdf?chaveDeAcessoNaoAutenticado=97827de5f831bdf92b6c6bd603308190ea2769c6</t>
+  </si>
+  <si>
+    <t>https://www.gov.br/saude/pt-br/assuntos/novo-pac-saude/unidades-basicas-de-saude/faq-ubs/analise-habilitacao-e-selecao-das-propostas/valores-para-construcao-de-nova-ubs</t>
+  </si>
+  <si>
+    <t>PORTE UBS</t>
+  </si>
+  <si>
+    <t>VALORES PARA CONSTRUÇÃO DE UBS - 2024 (R$)</t>
+  </si>
+  <si>
+    <t>Norte</t>
+  </si>
+  <si>
+    <t>Nordeste</t>
+  </si>
+  <si>
+    <t>Sudeste</t>
+  </si>
+  <si>
+    <t>Sul</t>
+  </si>
+  <si>
+    <t>Centro-Oeste</t>
+  </si>
+  <si>
+    <t>UBS I</t>
+  </si>
+  <si>
+    <t>R$ 1.887.023,00</t>
+  </si>
+  <si>
+    <t>R$ 1.816.494,00</t>
+  </si>
+  <si>
+    <t>R$ 2.012.825,00</t>
+  </si>
+  <si>
+    <t>R$ 2.026.110,00</t>
+  </si>
+  <si>
+    <t>R$ 1.881.388,00</t>
+  </si>
+  <si>
+    <t>UBS II</t>
+  </si>
+  <si>
+    <t>R$ 2.283.728,00</t>
+  </si>
+  <si>
+    <t>R$ 2.198.371,00</t>
+  </si>
+  <si>
+    <t>R$ 2.435.976,00</t>
+  </si>
+  <si>
+    <t>R$ 2.452.054,00</t>
+  </si>
+  <si>
+    <t>R$ 2.276.907,00</t>
+  </si>
+  <si>
+    <t>UBS III</t>
+  </si>
+  <si>
+    <t>R$ 2.592.535,00</t>
+  </si>
+  <si>
+    <t>R$ 2.495.636,00</t>
+  </si>
+  <si>
+    <t>R$ 2.765.371,00</t>
+  </si>
+  <si>
+    <t>R$ 2.783.622,00</t>
+  </si>
+  <si>
+    <t>R$ 2.584.792,00</t>
+  </si>
+  <si>
+    <t>UBS IV</t>
+  </si>
+  <si>
+    <t>R$ 4.960.637,00</t>
+  </si>
+  <si>
+    <t>R$ 4.775.227,00</t>
+  </si>
+  <si>
+    <t>R$ 5.291.345,00</t>
+  </si>
+  <si>
+    <t>R$ 5.326.268,00</t>
+  </si>
+  <si>
+    <t>R$ 4.945.820,00</t>
+  </si>
+  <si>
+    <t>UBS V</t>
+  </si>
+  <si>
+    <t>R$ 6.173.319,00</t>
+  </si>
+  <si>
+    <t>R$ 5.942.585,00</t>
+  </si>
+  <si>
+    <t>R$ 6.584.873,00</t>
+  </si>
+  <si>
+    <t>R$ 6.628.334,00</t>
+  </si>
+  <si>
+    <t>R$ 6.154.881,00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2270,10 +2397,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
+      <i/>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2302,31 +2437,53 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="Hiperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
+    <cellStyle name="Vírgula" xfId="3" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2678,11 +2835,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898BD5C2-36EA-49A0-935B-2C58D1998A71}">
-  <dimension ref="A1:F225"/>
+  <dimension ref="A1:G225"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5959,7 +6114,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>191</v>
       </c>
@@ -5976,7 +6131,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>192</v>
       </c>
@@ -5993,7 +6148,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>193</v>
       </c>
@@ -6010,7 +6165,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>194</v>
       </c>
@@ -6027,7 +6182,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>195</v>
       </c>
@@ -6044,7 +6199,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>196</v>
       </c>
@@ -6061,7 +6216,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>197</v>
       </c>
@@ -6078,7 +6233,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>198</v>
       </c>
@@ -6094,8 +6249,9 @@
       <c r="E200" s="1" t="s">
         <v>693</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G200" s="1"/>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>199</v>
       </c>
@@ -6111,8 +6267,9 @@
       <c r="E201" s="1" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G201" s="1"/>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>200</v>
       </c>
@@ -6128,8 +6285,9 @@
       <c r="E202" s="1" t="s">
         <v>679</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G202" s="1"/>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>201</v>
       </c>
@@ -6146,7 +6304,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>202</v>
       </c>
@@ -6163,7 +6321,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>203</v>
       </c>
@@ -6180,7 +6338,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>204</v>
       </c>
@@ -6197,7 +6355,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>205</v>
       </c>
@@ -6214,7 +6372,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>206</v>
       </c>
@@ -6528,27 +6686,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D57B64A-4341-4B2E-B8F0-85F35BC09681}">
-  <dimension ref="B2:H18"/>
+  <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="11" t="s">
         <v>694</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
@@ -6577,34 +6735,38 @@
         <v>699</v>
       </c>
       <c r="C5" s="3">
-        <v>3000000</v>
+        <f>E39</f>
+        <v>3818078</v>
       </c>
       <c r="D5" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>701</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <f>I_*(r_*(1+r_)^n_)/((1+r_)^n_-1)</f>
-        <v>352378.8743176373</v>
-      </c>
-      <c r="D6" s="9" t="s">
+        <v>448470.00923231198</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
+      <c r="B8" s="9"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="10"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="5" t="s">
+        <v>718</v>
+      </c>
       <c r="D9" t="s">
         <v>714</v>
       </c>
@@ -6622,7 +6784,7 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>708</v>
       </c>
       <c r="C10" s="3">
@@ -6650,7 +6812,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>709</v>
       </c>
       <c r="C11" s="3">
@@ -6678,7 +6840,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>715</v>
       </c>
       <c r="C12" s="3">
@@ -6706,31 +6868,31 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="10"/>
+      <c r="B13" s="9"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>707</v>
       </c>
       <c r="C17" s="3">
         <f>Ian</f>
-        <v>352378.8743176373</v>
+        <v>448470.00923231198</v>
       </c>
       <c r="D17" t="str">
         <f>D6</f>
         <v>Investimento anualizado da nova UBS</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>706</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <f>SUM(C10:C12)</f>
         <v>2707515.5555555555</v>
       </c>
@@ -6738,11 +6900,204 @@
         <v>705</v>
       </c>
     </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>716</v>
+      </c>
+      <c r="C20">
+        <f>ROUND(SUM(F10:F12)/(3*3000),0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>717</v>
+      </c>
+      <c r="C21" s="3">
+        <v>100000</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>718</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="14" t="s">
+        <v>721</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>722</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="13"/>
+      <c r="C26" s="14" t="s">
+        <v>723</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>724</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>725</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>726</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="14" t="s">
+        <v>728</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>729</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>730</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>731</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>732</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
+        <v>734</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>735</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>736</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>737</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>738</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="14" t="s">
+        <v>740</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>741</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>742</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>743</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>744</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>745</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
+        <v>746</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>747</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>748</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>749</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>750</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
+        <v>752</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>753</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>754</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>755</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>756</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="16" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="17">
+        <v>2012825</v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="18">
+        <v>2435976</v>
+      </c>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="18">
+        <v>2765371</v>
+      </c>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="18">
+        <v>5291345</v>
+      </c>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="18">
+        <v>6584873</v>
+      </c>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="19">
+        <f>AVERAGE(E34:E38)</f>
+        <v>3818078</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="C25:G25"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B32" r:id="rId1" xr:uid="{20B876B4-C3B4-4CCF-BF03-E5F115DF2520}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>